<commit_message>
UI Improved and working
</commit_message>
<xml_diff>
--- a/Scrum/Proyect/Sprint-backlog-template (1).xlsx
+++ b/Scrum/Proyect/Sprint-backlog-template (1).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Backlog Item</t>
   </si>
@@ -45,12 +45,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Sprint Backlog Template</t>
-  </si>
-  <si>
-    <t>Create a Sprint Backlog in Smartsheet</t>
   </si>
   <si>
     <t>Extract MLB Stats</t>
@@ -140,7 +134,25 @@
     <t>Actual remaining hours</t>
   </si>
   <si>
-    <t>Pending</t>
+    <t>Save data in database</t>
+  </si>
+  <si>
+    <t>Ezequiel says priority is to save in database</t>
+  </si>
+  <si>
+    <t>Sprint Backlog</t>
+  </si>
+  <si>
+    <t>Pending 23</t>
+  </si>
+  <si>
+    <t>Pending 24</t>
+  </si>
+  <si>
+    <t>Day 26</t>
+  </si>
+  <si>
+    <t>Day 27</t>
   </si>
 </sst>
 </file>
@@ -150,6 +162,13 @@
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -191,13 +210,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
@@ -206,7 +218,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,12 +262,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -298,14 +317,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -321,8 +341,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -332,30 +352,34 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="3"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="4"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
+  <cellStyles count="6">
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="5" builtinId="43"/>
+    <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -412,7 +436,16 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Sprint Burndown </a:t>
+              <a:t>Sprint Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -485,9 +518,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$6:$M$6</c:f>
+              <c:f>Sheet1!$F$6:$O$6</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Day 21</c:v>
                 </c:pt>
@@ -504,12 +537,18 @@
                   <c:v>Day 25</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Day 26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 27</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>Day 28</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Day 29</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Sprint Review</c:v>
                 </c:pt>
               </c:strCache>
@@ -517,33 +556,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$35:$M$35</c:f>
+              <c:f>Sheet1!$E$35:$O$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>84</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>69</c:v>
+                <c:pt idx="10">
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -589,9 +622,9 @@
           </c:trendline>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$6:$M$6</c:f>
+              <c:f>Sheet1!$F$6:$O$6</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Day 21</c:v>
                 </c:pt>
@@ -608,12 +641,18 @@
                   <c:v>Day 25</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Day 26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 27</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>Day 28</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Day 29</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Sprint Review</c:v>
                 </c:pt>
               </c:strCache>
@@ -626,31 +665,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>84</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>76</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>68</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>52</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -666,11 +705,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-585089200"/>
-        <c:axId val="-585090832"/>
+        <c:axId val="-580474160"/>
+        <c:axId val="-580473616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-585089200"/>
+        <c:axId val="-580474160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -712,7 +751,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-585090832"/>
+        <c:crossAx val="-580473616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -720,7 +759,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-585090832"/>
+        <c:axId val="-580473616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,7 +809,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-585089200"/>
+        <c:crossAx val="-580474160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1370,16 +1409,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>174625</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3143250</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>60325</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>3175</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1396,82 +1435,6 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>133640</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1028699</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>139699</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10230140" y="241300"/>
-          <a:ext cx="2546059" cy="571499"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>990600</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>49524</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>796925</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="990600" y="8723624"/>
-          <a:ext cx="16967200" cy="5030476"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1799,10 +1762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC138"/>
+  <dimension ref="A1:AE138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G40" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1810,12 +1773,12 @@
     <col min="1" max="1" width="53.5" customWidth="1"/>
     <col min="2" max="2" width="11.625" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.125" customWidth="1"/>
-    <col min="4" max="4" width="24.625" customWidth="1"/>
+    <col min="4" max="4" width="37" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
     <col min="11" max="11" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="6"/>
       <c r="C1" s="5"/>
@@ -1844,7 +1807,7 @@
       <c r="Z1" s="5"/>
       <c r="AA1" s="5"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="5"/>
@@ -1873,9 +1836,9 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
     </row>
-    <row r="3" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="5"/>
@@ -1904,7 +1867,7 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="5"/>
@@ -1933,7 +1896,7 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="5"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="5"/>
@@ -1962,7 +1925,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
     </row>
-    <row r="6" spans="1:29" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1979,35 +1942,41 @@
         <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="K6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
+      <c r="P6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
@@ -2020,10 +1989,12 @@
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
       <c r="AC6" s="5"/>
-    </row>
-    <row r="7" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+    </row>
+    <row r="7" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="8">
         <v>8</v>
@@ -2040,9 +2011,9 @@
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
@@ -2055,29 +2026,31 @@
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
       <c r="AC7" s="5"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="17">
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14">
         <v>10</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
@@ -2090,10 +2063,12 @@
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
       <c r="AC8" s="5"/>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD8" s="5"/>
+      <c r="AE8" s="5"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="13"/>
@@ -2110,15 +2085,17 @@
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="14">
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14">
         <v>4</v>
       </c>
-      <c r="N9" s="14">
+      <c r="P9" s="14">
         <v>0</v>
       </c>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
+      <c r="Q9" s="14">
+        <v>0</v>
+      </c>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
@@ -2131,10 +2108,12 @@
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
       <c r="AC9" s="5"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD9" s="5"/>
+      <c r="AE9" s="5"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="13"/>
@@ -2151,15 +2130,17 @@
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
-      <c r="M10" s="14">
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14">
         <v>2</v>
       </c>
-      <c r="N10" s="14">
+      <c r="P10" s="14">
         <v>0</v>
       </c>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
+      <c r="Q10" s="14">
+        <v>0</v>
+      </c>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
@@ -2172,10 +2153,12 @@
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
       <c r="AC10" s="5"/>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="5"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="13"/>
@@ -2193,12 +2176,14 @@
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
-      <c r="N11" s="14">
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14">
         <v>0</v>
       </c>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
+      <c r="Q11" s="14">
+        <v>0</v>
+      </c>
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
       <c r="T11" s="5"/>
@@ -2211,10 +2196,12 @@
       <c r="AA11" s="5"/>
       <c r="AB11" s="5"/>
       <c r="AC11" s="5"/>
-    </row>
-    <row r="12" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AD11" s="5"/>
+      <c r="AE11" s="5"/>
+    </row>
+    <row r="12" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="8">
         <v>1</v>
@@ -2231,9 +2218,9 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
@@ -2246,34 +2233,39 @@
       <c r="AA12" s="5"/>
       <c r="AB12" s="5"/>
       <c r="AC12" s="5"/>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4">
+      <c r="AD12" s="5"/>
+      <c r="AE12" s="5"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="19">
         <v>8</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4">
-        <f>E13</f>
-        <v>8</v>
-      </c>
-      <c r="N13" s="4">
-        <v>8</v>
-      </c>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19">
+        <v>0</v>
+      </c>
+      <c r="P13" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="19">
+        <v>0</v>
+      </c>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
@@ -2286,34 +2278,39 @@
       <c r="AA13" s="5"/>
       <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
-    </row>
-    <row r="14" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4">
+      <c r="AD13" s="5"/>
+      <c r="AE13" s="5"/>
+    </row>
+    <row r="14" spans="1:31" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="19">
         <v>7</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4">
-        <f t="shared" ref="M14:N35" si="0">E14</f>
-        <v>7</v>
-      </c>
-      <c r="N14" s="4">
-        <v>7</v>
-      </c>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19">
+        <v>0</v>
+      </c>
+      <c r="P14" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="19">
+        <v>0</v>
+      </c>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
@@ -2326,31 +2323,36 @@
       <c r="AA14" s="5"/>
       <c r="AB14" s="5"/>
       <c r="AC14" s="5"/>
-    </row>
-    <row r="15" spans="1:29" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21">
-        <f t="shared" si="0"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="5"/>
+    </row>
+    <row r="15" spans="1:31" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17">
+        <f>E15</f>
         <v>0</v>
       </c>
-      <c r="N15" s="21">
-        <f t="shared" si="0"/>
+      <c r="P15" s="17">
+        <f>F15</f>
         <v>0</v>
       </c>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
+      <c r="Q15" s="17">
+        <f>G15</f>
+        <v>0</v>
+      </c>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
       <c r="T15" s="5"/>
@@ -2363,31 +2365,36 @@
       <c r="AA15" s="5"/>
       <c r="AB15" s="5"/>
       <c r="AC15" s="5"/>
-    </row>
-    <row r="16" spans="1:29" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21">
-        <f t="shared" si="0"/>
+      <c r="AD15" s="5"/>
+      <c r="AE15" s="5"/>
+    </row>
+    <row r="16" spans="1:31" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17">
+        <f>E16</f>
         <v>0</v>
       </c>
-      <c r="N16" s="21">
-        <f t="shared" si="0"/>
+      <c r="P16" s="17">
+        <f>F16</f>
         <v>0</v>
       </c>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
+      <c r="Q16" s="17">
+        <f>G16</f>
+        <v>0</v>
+      </c>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
@@ -2400,10 +2407,12 @@
       <c r="AA16" s="5"/>
       <c r="AB16" s="5"/>
       <c r="AC16" s="5"/>
-    </row>
-    <row r="17" spans="1:29" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="AD16" s="5"/>
+      <c r="AE16" s="5"/>
+    </row>
+    <row r="17" spans="1:31" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="8">
         <v>5</v>
@@ -2418,17 +2427,20 @@
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
-      <c r="M17" s="4">
-        <f t="shared" si="0"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="4">
+        <f>E17</f>
         <v>0</v>
       </c>
-      <c r="N17" s="4">
-        <f t="shared" si="0"/>
+      <c r="P17" s="4">
+        <f>F17</f>
         <v>0</v>
       </c>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
+      <c r="Q17" s="4">
+        <f>G17</f>
+        <v>0</v>
+      </c>
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
@@ -2441,34 +2453,40 @@
       <c r="AA17" s="5"/>
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
-    </row>
-    <row r="18" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="4">
+      <c r="AD17" s="5"/>
+      <c r="AE17" s="5"/>
+    </row>
+    <row r="18" spans="1:31" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="21">
         <v>8</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4">
-        <f t="shared" si="0"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21">
+        <f>E18</f>
         <v>8</v>
       </c>
-      <c r="N18" s="4">
-        <v>8</v>
-      </c>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
+      <c r="P18" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="21">
+        <v>0</v>
+      </c>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
@@ -2481,31 +2499,36 @@
       <c r="AA18" s="5"/>
       <c r="AB18" s="5"/>
       <c r="AC18" s="5"/>
-    </row>
-    <row r="19" spans="1:29" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21">
-        <f t="shared" si="0"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="5"/>
+    </row>
+    <row r="19" spans="1:31" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17">
+        <f>E19</f>
         <v>0</v>
       </c>
-      <c r="N19" s="21">
-        <f t="shared" si="0"/>
+      <c r="P19" s="17">
+        <f>F19</f>
         <v>0</v>
       </c>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
+      <c r="Q19" s="17">
+        <f>G19</f>
+        <v>0</v>
+      </c>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
@@ -2518,31 +2541,36 @@
       <c r="AA19" s="5"/>
       <c r="AB19" s="5"/>
       <c r="AC19" s="5"/>
-    </row>
-    <row r="20" spans="1:29" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21">
-        <f t="shared" si="0"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="5"/>
+    </row>
+    <row r="20" spans="1:31" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17">
+        <f>E20</f>
         <v>0</v>
       </c>
-      <c r="N20" s="21">
-        <f t="shared" si="0"/>
+      <c r="P20" s="17">
+        <f>F20</f>
         <v>0</v>
       </c>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
+      <c r="Q20" s="17">
+        <f>G20</f>
+        <v>0</v>
+      </c>
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
@@ -2555,31 +2583,36 @@
       <c r="AA20" s="5"/>
       <c r="AB20" s="5"/>
       <c r="AC20" s="5"/>
-    </row>
-    <row r="21" spans="1:29" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21">
-        <f t="shared" si="0"/>
+      <c r="AD20" s="5"/>
+      <c r="AE20" s="5"/>
+    </row>
+    <row r="21" spans="1:31" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17">
+        <f>E21</f>
         <v>0</v>
       </c>
-      <c r="N21" s="21">
-        <f t="shared" si="0"/>
+      <c r="P21" s="17">
+        <f>F21</f>
         <v>0</v>
       </c>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
+      <c r="Q21" s="17">
+        <f>G21</f>
+        <v>0</v>
+      </c>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
@@ -2592,10 +2625,12 @@
       <c r="AA21" s="5"/>
       <c r="AB21" s="5"/>
       <c r="AC21" s="5"/>
-    </row>
-    <row r="22" spans="1:29" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="AD21" s="5"/>
+      <c r="AE21" s="5"/>
+    </row>
+    <row r="22" spans="1:31" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B22" s="8">
         <v>8</v>
@@ -2610,17 +2645,20 @@
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
-      <c r="M22" s="4">
-        <f t="shared" si="0"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="4">
+        <f>E22</f>
         <v>0</v>
       </c>
-      <c r="N22" s="4">
-        <f t="shared" si="0"/>
+      <c r="P22" s="4">
+        <f>F22</f>
         <v>0</v>
       </c>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
+      <c r="Q22" s="4">
+        <f>G22</f>
+        <v>0</v>
+      </c>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
@@ -2633,10 +2671,12 @@
       <c r="AA22" s="5"/>
       <c r="AB22" s="5"/>
       <c r="AC22" s="5"/>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD22" s="5"/>
+      <c r="AE22" s="5"/>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="13"/>
@@ -2653,16 +2693,18 @@
       <c r="J23" s="14"/>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
-      <c r="M23" s="14">
-        <f t="shared" si="0"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14">
+        <f>E23</f>
         <v>8</v>
       </c>
-      <c r="N23" s="14">
+      <c r="P23" s="14">
         <v>0</v>
       </c>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
+      <c r="Q23" s="14">
+        <v>0</v>
+      </c>
       <c r="R23" s="5"/>
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
@@ -2675,10 +2717,12 @@
       <c r="AA23" s="5"/>
       <c r="AB23" s="5"/>
       <c r="AC23" s="5"/>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD23" s="5"/>
+      <c r="AE23" s="5"/>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="13"/>
@@ -2695,16 +2739,18 @@
       <c r="J24" s="14"/>
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
-      <c r="M24" s="14">
-        <f t="shared" si="0"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14">
+        <f>E24</f>
         <v>8</v>
       </c>
-      <c r="N24" s="14">
+      <c r="P24" s="14">
         <v>0</v>
       </c>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
+      <c r="Q24" s="14">
+        <v>0</v>
+      </c>
       <c r="R24" s="5"/>
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
@@ -2717,10 +2763,12 @@
       <c r="AA24" s="5"/>
       <c r="AB24" s="5"/>
       <c r="AC24" s="5"/>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD24" s="5"/>
+      <c r="AE24" s="5"/>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="13"/>
@@ -2737,16 +2785,18 @@
       <c r="J25" s="14"/>
       <c r="K25" s="14"/>
       <c r="L25" s="14"/>
-      <c r="M25" s="14">
-        <f t="shared" si="0"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14">
+        <f>E25</f>
         <v>8</v>
       </c>
-      <c r="N25" s="14">
+      <c r="P25" s="14">
         <v>0</v>
       </c>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
+      <c r="Q25" s="14">
+        <v>0</v>
+      </c>
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
@@ -2759,10 +2809,12 @@
       <c r="AA25" s="5"/>
       <c r="AB25" s="5"/>
       <c r="AC25" s="5"/>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD25" s="5"/>
+      <c r="AE25" s="5"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B26" s="14">
         <v>8</v>
@@ -2781,16 +2833,18 @@
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
       <c r="L26" s="14"/>
-      <c r="M26" s="14">
-        <f t="shared" si="0"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14">
+        <f>E26</f>
         <v>8</v>
       </c>
-      <c r="N26" s="14">
+      <c r="P26" s="14">
         <v>0</v>
       </c>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
+      <c r="Q26" s="14">
+        <v>0</v>
+      </c>
       <c r="R26" s="5"/>
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
@@ -2803,10 +2857,12 @@
       <c r="AA26" s="5"/>
       <c r="AB26" s="5"/>
       <c r="AC26" s="5"/>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="5"/>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" s="14">
         <v>8</v>
@@ -2823,17 +2879,20 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
-      <c r="M27" s="4">
-        <f t="shared" si="0"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4">
+        <f>E27</f>
         <v>0</v>
       </c>
-      <c r="N27" s="4">
-        <f t="shared" si="0"/>
+      <c r="P27" s="4">
+        <f>F27</f>
         <v>0</v>
       </c>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
+      <c r="Q27" s="4">
+        <f>G27</f>
+        <v>0</v>
+      </c>
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
@@ -2846,10 +2905,12 @@
       <c r="AA27" s="5"/>
       <c r="AB27" s="5"/>
       <c r="AC27" s="5"/>
-    </row>
-    <row r="28" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="5"/>
+    </row>
+    <row r="28" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B28" s="8">
         <v>3</v>
@@ -2864,17 +2925,20 @@
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
-      <c r="M28" s="4">
-        <f t="shared" si="0"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="4">
+        <f>E28</f>
         <v>0</v>
       </c>
-      <c r="N28" s="4">
-        <f t="shared" si="0"/>
+      <c r="P28" s="4">
+        <f>F28</f>
         <v>0</v>
       </c>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
+      <c r="Q28" s="4">
+        <f>G28</f>
+        <v>0</v>
+      </c>
       <c r="R28" s="5"/>
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
@@ -2887,10 +2951,12 @@
       <c r="AA28" s="5"/>
       <c r="AB28" s="5"/>
       <c r="AC28" s="5"/>
-    </row>
-    <row r="29" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="5"/>
+    </row>
+    <row r="29" spans="1:31" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
@@ -2905,16 +2971,18 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
-      <c r="M29" s="4">
-        <f t="shared" si="0"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4">
+        <f>E29</f>
         <v>8</v>
       </c>
-      <c r="N29" s="4">
+      <c r="P29" s="4">
         <v>8</v>
       </c>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
+      <c r="Q29" s="4">
+        <v>8</v>
+      </c>
       <c r="R29" s="5"/>
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
@@ -2927,31 +2995,36 @@
       <c r="AA29" s="5"/>
       <c r="AB29" s="5"/>
       <c r="AC29" s="5"/>
-    </row>
-    <row r="30" spans="1:29" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="20"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21">
-        <f t="shared" si="0"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29" s="5"/>
+    </row>
+    <row r="30" spans="1:31" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="16"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17">
+        <f>E30</f>
         <v>0</v>
       </c>
-      <c r="N30" s="21">
-        <f t="shared" si="0"/>
+      <c r="P30" s="17">
+        <f>F30</f>
         <v>0</v>
       </c>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
+      <c r="Q30" s="17">
+        <f>G30</f>
+        <v>0</v>
+      </c>
       <c r="R30" s="5"/>
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
@@ -2964,31 +3037,36 @@
       <c r="AA30" s="5"/>
       <c r="AB30" s="5"/>
       <c r="AC30" s="5"/>
-    </row>
-    <row r="31" spans="1:29" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="20"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21">
-        <f t="shared" si="0"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30" s="5"/>
+    </row>
+    <row r="31" spans="1:31" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="16"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17">
+        <f>E31</f>
         <v>0</v>
       </c>
-      <c r="N31" s="21">
-        <f t="shared" si="0"/>
+      <c r="P31" s="17">
+        <f>F31</f>
         <v>0</v>
       </c>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
+      <c r="Q31" s="17">
+        <f>G31</f>
+        <v>0</v>
+      </c>
       <c r="R31" s="5"/>
       <c r="S31" s="5"/>
       <c r="T31" s="5"/>
@@ -3001,10 +3079,12 @@
       <c r="AA31" s="5"/>
       <c r="AB31" s="5"/>
       <c r="AC31" s="5"/>
-    </row>
-    <row r="32" spans="1:29" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AD31" s="5"/>
+      <c r="AE31" s="5"/>
+    </row>
+    <row r="32" spans="1:31" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
@@ -3017,17 +3097,20 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="4">
-        <f t="shared" si="0"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4">
+        <f>E32</f>
         <v>0</v>
       </c>
-      <c r="N32" s="4">
-        <f t="shared" si="0"/>
+      <c r="P32" s="4">
+        <f>F32</f>
         <v>0</v>
       </c>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
+      <c r="Q32" s="4">
+        <f>G32</f>
+        <v>0</v>
+      </c>
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
       <c r="T32" s="5"/>
@@ -3040,10 +3123,12 @@
       <c r="AA32" s="5"/>
       <c r="AB32" s="5"/>
       <c r="AC32" s="5"/>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD32" s="5"/>
+      <c r="AE32" s="5"/>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
@@ -3056,17 +3141,20 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
-      <c r="M33" s="4">
-        <f t="shared" si="0"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4">
+        <f>E33</f>
         <v>0</v>
       </c>
-      <c r="N33" s="4">
-        <f t="shared" si="0"/>
+      <c r="P33" s="4">
+        <f>F33</f>
         <v>0</v>
       </c>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
+      <c r="Q33" s="4">
+        <f>G33</f>
+        <v>0</v>
+      </c>
       <c r="R33" s="5"/>
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
@@ -3079,13 +3167,19 @@
       <c r="AA33" s="5"/>
       <c r="AB33" s="5"/>
       <c r="AC33" s="5"/>
-    </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
+      <c r="AD33" s="5"/>
+      <c r="AE33" s="5"/>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4">
+        <v>8</v>
+      </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
@@ -3093,17 +3187,18 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
-      <c r="M34" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N34" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O34" s="5"/>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4">
+        <f>E34</f>
+        <v>8</v>
+      </c>
+      <c r="P34" s="4">
+        <v>8</v>
+      </c>
+      <c r="Q34" s="4">
+        <v>8</v>
+      </c>
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
@@ -3116,56 +3211,55 @@
       <c r="AA34" s="5"/>
       <c r="AB34" s="5"/>
       <c r="AC34" s="5"/>
-    </row>
-    <row r="35" spans="1:29" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD34" s="5"/>
+      <c r="AE34" s="5"/>
+    </row>
+    <row r="35" spans="1:31" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E35" s="11">
         <f>SUM(E7:E34)</f>
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F35" s="11">
-        <f>SUM(M8:M34)-SUM(F8:F34)</f>
-        <v>41</v>
+        <f>SUM(O8:O34)-SUM(F8:F34)</f>
+        <v>34</v>
       </c>
       <c r="G35" s="11">
         <f>F35-SUM(G8:G34)</f>
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H35" s="11">
-        <f>G35-8</f>
-        <v>26</v>
+        <f>P35</f>
+        <v>16</v>
       </c>
       <c r="I35" s="11">
-        <f>H35-8</f>
-        <v>18</v>
-      </c>
-      <c r="J35" s="11">
-        <f>I35-8</f>
-        <v>10</v>
-      </c>
-      <c r="K35" s="11">
-        <f>J35-8</f>
-        <v>2</v>
-      </c>
+        <f>P35</f>
+        <v>16</v>
+      </c>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
       <c r="L35" s="11"/>
-      <c r="M35" s="4">
-        <f>SUM(M7:M34)</f>
-        <v>69</v>
-      </c>
-      <c r="N35" s="4">
-        <f>SUM(N7:N34)</f>
-        <v>31</v>
-      </c>
-      <c r="O35" s="5"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="5"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="4">
+        <f>SUM(O7:O34)</f>
+        <v>62</v>
+      </c>
+      <c r="P35" s="4">
+        <f>SUM(P7:P34)</f>
+        <v>16</v>
+      </c>
+      <c r="Q35" s="4">
+        <f>SUM(Q7:Q34)</f>
+        <v>16</v>
+      </c>
       <c r="R35" s="5"/>
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
@@ -3178,53 +3272,55 @@
       <c r="AA35" s="5"/>
       <c r="AB35" s="5"/>
       <c r="AC35" s="5"/>
-    </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD35" s="5"/>
+      <c r="AE35" s="5"/>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="6"/>
       <c r="C36" s="5"/>
       <c r="D36" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E36" s="5">
         <f>SUM(E8:E34)</f>
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F36" s="5">
         <f>E36-8</f>
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="G36" s="5">
         <f>F36-8</f>
+        <v>76</v>
+      </c>
+      <c r="H36" s="5">
+        <f t="shared" ref="H36:N36" si="0">G36-8</f>
         <v>68</v>
       </c>
-      <c r="H36" s="5">
-        <f t="shared" ref="H36:N36" si="1">G36-8</f>
+      <c r="I36" s="5">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="I36" s="5">
-        <f t="shared" si="1"/>
+      <c r="J36" s="5">
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="J36" s="5">
-        <f t="shared" si="1"/>
+      <c r="K36" s="5">
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="K36" s="5">
-        <f t="shared" si="1"/>
+      <c r="L36" s="5">
+        <f t="shared" si="0"/>
         <v>36</v>
-      </c>
-      <c r="L36" s="5">
-        <f t="shared" si="1"/>
-        <v>28</v>
       </c>
       <c r="M36" s="5">
         <f>L36-8</f>
+        <v>28</v>
+      </c>
+      <c r="N36" s="5">
+        <f t="shared" si="0"/>
         <v>20</v>
-      </c>
-      <c r="N36" s="5">
-        <f t="shared" si="1"/>
-        <v>12</v>
       </c>
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
@@ -3240,29 +3336,27 @@
       <c r="Z36" s="5"/>
       <c r="AA36" s="5"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="19"/>
-      <c r="R37" s="19"/>
-      <c r="S37" s="19"/>
-      <c r="T37" s="19"/>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
+      <c r="N37" s="22"/>
+      <c r="O37" s="22"/>
+      <c r="P37" s="22"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22"/>
+      <c r="S37" s="22"/>
+      <c r="T37" s="22"/>
       <c r="U37" s="5"/>
       <c r="V37" s="5"/>
       <c r="W37" s="5"/>
@@ -3271,27 +3365,27 @@
       <c r="Z37" s="5"/>
       <c r="AA37" s="5"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="19"/>
-      <c r="R38" s="19"/>
-      <c r="S38" s="19"/>
-      <c r="T38" s="19"/>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="22"/>
+      <c r="O38" s="22"/>
+      <c r="P38" s="22"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="22"/>
+      <c r="S38" s="22"/>
+      <c r="T38" s="22"/>
       <c r="U38" s="5"/>
       <c r="V38" s="5"/>
       <c r="W38" s="5"/>
@@ -3300,27 +3394,27 @@
       <c r="Z38" s="5"/>
       <c r="AA38" s="5"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="19"/>
-      <c r="O39" s="19"/>
-      <c r="P39" s="19"/>
-      <c r="Q39" s="19"/>
-      <c r="R39" s="19"/>
-      <c r="S39" s="19"/>
-      <c r="T39" s="19"/>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A39" s="22"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="22"/>
+      <c r="M39" s="22"/>
+      <c r="N39" s="22"/>
+      <c r="O39" s="22"/>
+      <c r="P39" s="22"/>
+      <c r="Q39" s="22"/>
+      <c r="R39" s="22"/>
+      <c r="S39" s="22"/>
+      <c r="T39" s="22"/>
       <c r="U39" s="5"/>
       <c r="V39" s="5"/>
       <c r="W39" s="5"/>
@@ -3329,27 +3423,27 @@
       <c r="Z39" s="5"/>
       <c r="AA39" s="5"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="19"/>
-      <c r="M40" s="19"/>
-      <c r="N40" s="19"/>
-      <c r="O40" s="19"/>
-      <c r="P40" s="19"/>
-      <c r="Q40" s="19"/>
-      <c r="R40" s="19"/>
-      <c r="S40" s="19"/>
-      <c r="T40" s="19"/>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A40" s="22"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="22"/>
+      <c r="N40" s="22"/>
+      <c r="O40" s="22"/>
+      <c r="P40" s="22"/>
+      <c r="Q40" s="22"/>
+      <c r="R40" s="22"/>
+      <c r="S40" s="22"/>
+      <c r="T40" s="22"/>
       <c r="U40" s="5"/>
       <c r="V40" s="5"/>
       <c r="W40" s="5"/>
@@ -3358,27 +3452,27 @@
       <c r="Z40" s="5"/>
       <c r="AA40" s="5"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="19"/>
-      <c r="O41" s="19"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="19"/>
-      <c r="R41" s="19"/>
-      <c r="S41" s="19"/>
-      <c r="T41" s="19"/>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A41" s="22"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
+      <c r="L41" s="22"/>
+      <c r="M41" s="22"/>
+      <c r="N41" s="22"/>
+      <c r="O41" s="22"/>
+      <c r="P41" s="22"/>
+      <c r="Q41" s="22"/>
+      <c r="R41" s="22"/>
+      <c r="S41" s="22"/>
+      <c r="T41" s="22"/>
       <c r="U41" s="5"/>
       <c r="V41" s="5"/>
       <c r="W41" s="5"/>
@@ -3387,27 +3481,27 @@
       <c r="Z41" s="5"/>
       <c r="AA41" s="5"/>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
-      <c r="N42" s="19"/>
-      <c r="O42" s="19"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="19"/>
-      <c r="R42" s="19"/>
-      <c r="S42" s="19"/>
-      <c r="T42" s="19"/>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A42" s="22"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="22"/>
+      <c r="N42" s="22"/>
+      <c r="O42" s="22"/>
+      <c r="P42" s="22"/>
+      <c r="Q42" s="22"/>
+      <c r="R42" s="22"/>
+      <c r="S42" s="22"/>
+      <c r="T42" s="22"/>
       <c r="U42" s="5"/>
       <c r="V42" s="5"/>
       <c r="W42" s="5"/>
@@ -3416,7 +3510,7 @@
       <c r="Z42" s="5"/>
       <c r="AA42" s="5"/>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="6"/>
       <c r="C43" s="5"/>
@@ -3445,7 +3539,7 @@
       <c r="Z43" s="5"/>
       <c r="AA43" s="5"/>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="6"/>
       <c r="C44" s="5"/>
@@ -3474,7 +3568,7 @@
       <c r="Z44" s="5"/>
       <c r="AA44" s="5"/>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="6"/>
       <c r="C45" s="5"/>
@@ -3503,7 +3597,7 @@
       <c r="Z45" s="5"/>
       <c r="AA45" s="5"/>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="6"/>
       <c r="C46" s="5"/>
@@ -3532,7 +3626,7 @@
       <c r="Z46" s="5"/>
       <c r="AA46" s="5"/>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="6"/>
       <c r="C47" s="5"/>
@@ -3561,7 +3655,7 @@
       <c r="Z47" s="5"/>
       <c r="AA47" s="5"/>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="6"/>
       <c r="C48" s="5"/>
@@ -6205,130 +6299,10 @@
     <mergeCell ref="A37:T42"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A37" r:id="rId1"/>
-    <hyperlink ref="B37" r:id="rId2" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="C37" r:id="rId3" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="D37" r:id="rId4" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="E37" r:id="rId5" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="F37" r:id="rId6" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="G37" r:id="rId7" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="H37" r:id="rId8" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="I37" r:id="rId9" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="J37" r:id="rId10" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="K37" r:id="rId11" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="L37" r:id="rId12" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="M37" r:id="rId13" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="N37" r:id="rId14" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="O37" r:id="rId15" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="P37" r:id="rId16" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="Q37" r:id="rId17" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="R37" r:id="rId18" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="S37" r:id="rId19" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="T37" r:id="rId20" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="A38" r:id="rId21" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="B38" r:id="rId22" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="C38" r:id="rId23" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="D38" r:id="rId24" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="E38" r:id="rId25" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="F38" r:id="rId26" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="G38" r:id="rId27" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="H38" r:id="rId28" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="I38" r:id="rId29" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="J38" r:id="rId30" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="K38" r:id="rId31" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="L38" r:id="rId32" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="M38" r:id="rId33" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="N38" r:id="rId34" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="O38" r:id="rId35" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="P38" r:id="rId36" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="Q38" r:id="rId37" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="R38" r:id="rId38" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="S38" r:id="rId39" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="T38" r:id="rId40" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="A39" r:id="rId41" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="B39" r:id="rId42" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="C39" r:id="rId43" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="D39" r:id="rId44" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="E39" r:id="rId45" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="F39" r:id="rId46" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="G39" r:id="rId47" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="H39" r:id="rId48" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="I39" r:id="rId49" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="J39" r:id="rId50" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="K39" r:id="rId51" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="L39" r:id="rId52" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="M39" r:id="rId53" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="N39" r:id="rId54" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="O39" r:id="rId55" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="P39" r:id="rId56" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="Q39" r:id="rId57" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="R39" r:id="rId58" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="S39" r:id="rId59" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="T39" r:id="rId60" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="A40" r:id="rId61" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="B40" r:id="rId62" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="C40" r:id="rId63" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="D40" r:id="rId64" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="E40" r:id="rId65" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="F40" r:id="rId66" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="G40" r:id="rId67" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="H40" r:id="rId68" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="I40" r:id="rId69" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="J40" r:id="rId70" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="K40" r:id="rId71" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="L40" r:id="rId72" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="M40" r:id="rId73" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="N40" r:id="rId74" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="O40" r:id="rId75" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="P40" r:id="rId76" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="Q40" r:id="rId77" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="R40" r:id="rId78" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="S40" r:id="rId79" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="T40" r:id="rId80" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="A41" r:id="rId81" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="B41" r:id="rId82" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="C41" r:id="rId83" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="D41" r:id="rId84" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="E41" r:id="rId85" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="F41" r:id="rId86" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="G41" r:id="rId87" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="H41" r:id="rId88" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="I41" r:id="rId89" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="J41" r:id="rId90" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="K41" r:id="rId91" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="L41" r:id="rId92" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="M41" r:id="rId93" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="N41" r:id="rId94" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="O41" r:id="rId95" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="P41" r:id="rId96" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="Q41" r:id="rId97" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="R41" r:id="rId98" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="S41" r:id="rId99" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="T41" r:id="rId100" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="A42" r:id="rId101" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="B42" r:id="rId102" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="C42" r:id="rId103" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="D42" r:id="rId104" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="E42" r:id="rId105" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="F42" r:id="rId106" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="G42" r:id="rId107" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="H42" r:id="rId108" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="I42" r:id="rId109" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="J42" r:id="rId110" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="K42" r:id="rId111" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="L42" r:id="rId112" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="M42" r:id="rId113" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="N42" r:id="rId114" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="O42" r:id="rId115" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="P42" r:id="rId116" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="Q42" r:id="rId117" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="R42" r:id="rId118" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="S42" r:id="rId119" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="T42" r:id="rId120" display="Create a Sprint Backlog in Smartsheet"/>
-    <hyperlink ref="A26" r:id="rId121" display="http://www.covers.com/pageLoader/pageLoader.aspx?page=/data/mlb/matchups/g4_summary_12.html"/>
+    <hyperlink ref="A26" r:id="rId1" display="http://www.covers.com/pageLoader/pageLoader.aspx?page=/data/mlb/matchups/g4_summary_12.html"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId122"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
@@ -6343,7 +6317,7 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!E35:O35</xm:f>
+              <xm:f>Sheet1!E35:Q35</xm:f>
               <xm:sqref>D35</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>

</xml_diff>

<commit_message>
Loading all the next games that contains pitchers
</commit_message>
<xml_diff>
--- a/Scrum/Proyect/Sprint-backlog-template (1).xlsx
+++ b/Scrum/Proyect/Sprint-backlog-template (1).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Backlog Item</t>
   </si>
@@ -104,12 +104,6 @@
     <t>Link between the extracted data (New requirement)</t>
   </si>
   <si>
-    <t>Extras</t>
-  </si>
-  <si>
-    <t>Extract datatable by headers</t>
-  </si>
-  <si>
     <t>Day 21</t>
   </si>
   <si>
@@ -134,9 +128,6 @@
     <t>Actual remaining hours</t>
   </si>
   <si>
-    <t>Save data in database</t>
-  </si>
-  <si>
     <t>Ezequiel says priority is to save in database</t>
   </si>
   <si>
@@ -154,12 +145,30 @@
   <si>
     <t>Day 27</t>
   </si>
+  <si>
+    <t>Extras 6.</t>
+  </si>
+  <si>
+    <t>6.1 Extract datatable by headers</t>
+  </si>
+  <si>
+    <t>6.2 Save data in database</t>
+  </si>
+  <si>
+    <t>Pending 25</t>
+  </si>
+  <si>
+    <t>5.2 Do upsert</t>
+  </si>
+  <si>
+    <t>5.3 Load game hour</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -217,8 +226,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +293,11 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -317,15 +338,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -370,13 +392,18 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="20% - Accent4" xfId="4" builtinId="42"/>
     <cellStyle name="40% - Accent4" xfId="5" builtinId="43"/>
+    <cellStyle name="Accent3" xfId="6" builtinId="37"/>
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -705,11 +732,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-580474160"/>
-        <c:axId val="-580473616"/>
+        <c:axId val="-581620672"/>
+        <c:axId val="-581623392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-580474160"/>
+        <c:axId val="-581620672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,7 +778,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-580473616"/>
+        <c:crossAx val="-581623392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -759,7 +786,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-580473616"/>
+        <c:axId val="-581623392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -809,7 +836,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-580474160"/>
+        <c:crossAx val="-581620672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1764,8 +1791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="M47" sqref="M47"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1838,7 +1865,7 @@
     </row>
     <row r="3" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="5"/>
@@ -1942,42 +1969,44 @@
         <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="K6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="R6" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
@@ -2014,7 +2043,7 @@
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
-      <c r="R7" s="5"/>
+      <c r="R7" s="10"/>
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
@@ -2051,7 +2080,7 @@
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
-      <c r="R8" s="5"/>
+      <c r="R8" s="14"/>
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
@@ -2096,7 +2125,9 @@
       <c r="Q9" s="14">
         <v>0</v>
       </c>
-      <c r="R9" s="5"/>
+      <c r="R9" s="14">
+        <v>0</v>
+      </c>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
@@ -2141,7 +2172,9 @@
       <c r="Q10" s="14">
         <v>0</v>
       </c>
-      <c r="R10" s="5"/>
+      <c r="R10" s="14">
+        <v>0</v>
+      </c>
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
@@ -2184,7 +2217,9 @@
       <c r="Q11" s="14">
         <v>0</v>
       </c>
-      <c r="R11" s="5"/>
+      <c r="R11" s="14">
+        <v>0</v>
+      </c>
       <c r="S11" s="5"/>
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
@@ -2221,7 +2256,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
-      <c r="R12" s="5"/>
+      <c r="R12" s="10"/>
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
       <c r="U12" s="5"/>
@@ -2243,7 +2278,7 @@
       <c r="B13" s="19"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E13" s="19">
         <v>8</v>
@@ -2266,7 +2301,9 @@
       <c r="Q13" s="19">
         <v>0</v>
       </c>
-      <c r="R13" s="5"/>
+      <c r="R13" s="19">
+        <v>0</v>
+      </c>
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
       <c r="U13" s="5"/>
@@ -2288,7 +2325,7 @@
       <c r="B14" s="19"/>
       <c r="C14" s="18"/>
       <c r="D14" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E14" s="19">
         <v>7</v>
@@ -2311,7 +2348,9 @@
       <c r="Q14" s="19">
         <v>0</v>
       </c>
-      <c r="R14" s="5"/>
+      <c r="R14" s="19">
+        <v>0</v>
+      </c>
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
       <c r="U14" s="5"/>
@@ -2342,18 +2381,21 @@
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
       <c r="O15" s="17">
-        <f>E15</f>
+        <f t="shared" ref="O15:R17" si="0">E15</f>
         <v>0</v>
       </c>
       <c r="P15" s="17">
-        <f>F15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q15" s="17">
-        <f>G15</f>
-        <v>0</v>
-      </c>
-      <c r="R15" s="5"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="S15" s="5"/>
       <c r="T15" s="5"/>
       <c r="U15" s="5"/>
@@ -2384,18 +2426,21 @@
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
       <c r="O16" s="17">
-        <f>E16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P16" s="17">
-        <f>F16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q16" s="17">
-        <f>G16</f>
-        <v>0</v>
-      </c>
-      <c r="R16" s="5"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
       <c r="U16" s="5"/>
@@ -2430,18 +2475,21 @@
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="4">
-        <f>E17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P17" s="4">
-        <f>F17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q17" s="4">
-        <f>G17</f>
-        <v>0</v>
-      </c>
-      <c r="R17" s="5"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
       <c r="U17" s="5"/>
@@ -2463,7 +2511,7 @@
       <c r="B18" s="21"/>
       <c r="C18" s="20"/>
       <c r="D18" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E18" s="21">
         <v>8</v>
@@ -2478,7 +2526,7 @@
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
       <c r="O18" s="21">
-        <f>E18</f>
+        <f t="shared" ref="O18:O34" si="1">E18</f>
         <v>8</v>
       </c>
       <c r="P18" s="21">
@@ -2487,7 +2535,9 @@
       <c r="Q18" s="21">
         <v>0</v>
       </c>
-      <c r="R18" s="5"/>
+      <c r="R18" s="21">
+        <v>0</v>
+      </c>
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
@@ -2518,18 +2568,21 @@
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
       <c r="O19" s="17">
-        <f>E19</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P19" s="17">
-        <f>F19</f>
+        <f t="shared" ref="P19:R22" si="2">F19</f>
         <v>0</v>
       </c>
       <c r="Q19" s="17">
-        <f>G19</f>
-        <v>0</v>
-      </c>
-      <c r="R19" s="5"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
       <c r="U19" s="5"/>
@@ -2560,18 +2613,21 @@
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
       <c r="O20" s="17">
-        <f>E20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P20" s="17">
-        <f>F20</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q20" s="17">
-        <f>G20</f>
-        <v>0</v>
-      </c>
-      <c r="R20" s="5"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
       <c r="U20" s="5"/>
@@ -2602,18 +2658,21 @@
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
       <c r="O21" s="17">
-        <f>E21</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P21" s="17">
-        <f>F21</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q21" s="17">
-        <f>G21</f>
-        <v>0</v>
-      </c>
-      <c r="R21" s="5"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R21" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
@@ -2648,18 +2707,21 @@
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
       <c r="O22" s="4">
-        <f>E22</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P22" s="4">
-        <f>F22</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q22" s="4">
-        <f>G22</f>
-        <v>0</v>
-      </c>
-      <c r="R22" s="5"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
@@ -2696,7 +2758,7 @@
       <c r="M23" s="14"/>
       <c r="N23" s="14"/>
       <c r="O23" s="14">
-        <f>E23</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="P23" s="14">
@@ -2705,7 +2767,9 @@
       <c r="Q23" s="14">
         <v>0</v>
       </c>
-      <c r="R23" s="5"/>
+      <c r="R23" s="14">
+        <v>0</v>
+      </c>
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
@@ -2742,7 +2806,7 @@
       <c r="M24" s="14"/>
       <c r="N24" s="14"/>
       <c r="O24" s="14">
-        <f>E24</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="P24" s="14">
@@ -2751,7 +2815,9 @@
       <c r="Q24" s="14">
         <v>0</v>
       </c>
-      <c r="R24" s="5"/>
+      <c r="R24" s="14">
+        <v>0</v>
+      </c>
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
       <c r="U24" s="5"/>
@@ -2788,7 +2854,7 @@
       <c r="M25" s="14"/>
       <c r="N25" s="14"/>
       <c r="O25" s="14">
-        <f>E25</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="P25" s="14">
@@ -2797,7 +2863,9 @@
       <c r="Q25" s="14">
         <v>0</v>
       </c>
-      <c r="R25" s="5"/>
+      <c r="R25" s="14">
+        <v>0</v>
+      </c>
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
       <c r="U25" s="5"/>
@@ -2836,7 +2904,7 @@
       <c r="M26" s="14"/>
       <c r="N26" s="14"/>
       <c r="O26" s="14">
-        <f>E26</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="P26" s="14">
@@ -2845,7 +2913,9 @@
       <c r="Q26" s="14">
         <v>0</v>
       </c>
-      <c r="R26" s="5"/>
+      <c r="R26" s="14">
+        <v>0</v>
+      </c>
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
       <c r="U26" s="5"/>
@@ -2882,18 +2952,21 @@
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4">
-        <f>E27</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P27" s="4">
-        <f>F27</f>
+        <f t="shared" ref="P27:R28" si="3">F27</f>
         <v>0</v>
       </c>
       <c r="Q27" s="4">
-        <f>G27</f>
-        <v>0</v>
-      </c>
-      <c r="R27" s="5"/>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R27" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
       <c r="U27" s="5"/>
@@ -2928,18 +3001,21 @@
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
       <c r="O28" s="4">
-        <f>E28</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P28" s="4">
-        <f>F28</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q28" s="4">
-        <f>G28</f>
-        <v>0</v>
-      </c>
-      <c r="R28" s="5"/>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R28" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
       <c r="U28" s="5"/>
@@ -2954,36 +3030,27 @@
       <c r="AD28" s="5"/>
       <c r="AE28" s="5"/>
     </row>
-    <row r="29" spans="1:31" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="4">
+      <c r="B29"/>
+      <c r="E29">
         <v>8</v>
       </c>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4">
-        <f>E29</f>
+      <c r="O29">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="P29" s="4">
+      <c r="P29">
         <v>8</v>
       </c>
-      <c r="Q29" s="4">
+      <c r="Q29">
         <v>8</v>
       </c>
-      <c r="R29" s="5"/>
+      <c r="R29">
+        <v>4</v>
+      </c>
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
       <c r="U29" s="5"/>
@@ -2998,34 +3065,26 @@
       <c r="AD29" s="5"/>
       <c r="AE29" s="5"/>
     </row>
-    <row r="30" spans="1:31" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="16"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17">
-        <f>E30</f>
-        <v>0</v>
-      </c>
-      <c r="P30" s="17">
-        <f>F30</f>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="17">
-        <f>G30</f>
-        <v>0</v>
-      </c>
-      <c r="R30" s="5"/>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30"/>
+      <c r="O30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <f t="shared" ref="P30:Q33" si="4">F30</f>
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>4</v>
+      </c>
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
@@ -3040,34 +3099,26 @@
       <c r="AD30" s="5"/>
       <c r="AE30" s="5"/>
     </row>
-    <row r="31" spans="1:31" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="16"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17">
-        <f>E31</f>
-        <v>0</v>
-      </c>
-      <c r="P31" s="17">
-        <f>F31</f>
-        <v>0</v>
-      </c>
-      <c r="Q31" s="17">
-        <f>G31</f>
-        <v>0</v>
-      </c>
-      <c r="R31" s="5"/>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31"/>
+      <c r="O31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
       <c r="S31" s="5"/>
       <c r="T31" s="5"/>
       <c r="U31" s="5"/>
@@ -3082,9 +3133,9 @@
       <c r="AD31" s="5"/>
       <c r="AE31" s="5"/>
     </row>
-    <row r="32" spans="1:31" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
@@ -3100,18 +3151,21 @@
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4">
-        <f>E32</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P32" s="4">
-        <f>F32</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q32" s="4">
-        <f>G32</f>
-        <v>0</v>
-      </c>
-      <c r="R32" s="5"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R32" s="4">
+        <f>H32</f>
+        <v>0</v>
+      </c>
       <c r="S32" s="5"/>
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
@@ -3128,7 +3182,7 @@
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
@@ -3144,18 +3198,21 @@
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4">
-        <f>E33</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P33" s="4">
-        <f>F33</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q33" s="4">
-        <f>G33</f>
-        <v>0</v>
-      </c>
-      <c r="R33" s="5"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R33" s="4">
+        <f>H33</f>
+        <v>0</v>
+      </c>
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
       <c r="U33" s="5"/>
@@ -3171,35 +3228,37 @@
       <c r="AE33" s="5"/>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="4">
+      <c r="A34" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="23"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="23">
         <v>8</v>
       </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4">
-        <f>E34</f>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="P34" s="4">
+      <c r="P34" s="23">
         <v>8</v>
       </c>
-      <c r="Q34" s="4">
+      <c r="Q34" s="23">
         <v>8</v>
       </c>
-      <c r="R34" s="5"/>
+      <c r="R34" s="23">
+        <v>0</v>
+      </c>
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
       <c r="U34" s="5"/>
@@ -3221,7 +3280,7 @@
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E35" s="11">
         <f>SUM(E7:E34)</f>
@@ -3260,7 +3319,10 @@
         <f>SUM(Q7:Q34)</f>
         <v>16</v>
       </c>
-      <c r="R35" s="5"/>
+      <c r="R35" s="4">
+        <f>SUM(R7:R34)</f>
+        <v>8</v>
+      </c>
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
       <c r="U35" s="5"/>
@@ -3295,23 +3357,23 @@
         <v>76</v>
       </c>
       <c r="H36" s="5">
-        <f t="shared" ref="H36:N36" si="0">G36-8</f>
+        <f t="shared" ref="H36:N36" si="5">G36-8</f>
         <v>68</v>
       </c>
       <c r="I36" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="J36" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>52</v>
       </c>
       <c r="K36" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>44</v>
       </c>
       <c r="L36" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="M36" s="5">
@@ -3319,7 +3381,7 @@
         <v>28</v>
       </c>
       <c r="N36" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="O36" s="5"/>
@@ -3337,26 +3399,26 @@
       <c r="AA36" s="5"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
-      <c r="O37" s="22"/>
-      <c r="P37" s="22"/>
-      <c r="Q37" s="22"/>
-      <c r="R37" s="22"/>
-      <c r="S37" s="22"/>
-      <c r="T37" s="22"/>
+      <c r="A37" s="24"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="24"/>
+      <c r="P37" s="24"/>
+      <c r="Q37" s="24"/>
+      <c r="R37" s="24"/>
+      <c r="S37" s="24"/>
+      <c r="T37" s="24"/>
       <c r="U37" s="5"/>
       <c r="V37" s="5"/>
       <c r="W37" s="5"/>
@@ -3366,26 +3428,26 @@
       <c r="AA37" s="5"/>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="22"/>
-      <c r="O38" s="22"/>
-      <c r="P38" s="22"/>
-      <c r="Q38" s="22"/>
-      <c r="R38" s="22"/>
-      <c r="S38" s="22"/>
-      <c r="T38" s="22"/>
+      <c r="A38" s="24"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
+      <c r="L38" s="24"/>
+      <c r="M38" s="24"/>
+      <c r="N38" s="24"/>
+      <c r="O38" s="24"/>
+      <c r="P38" s="24"/>
+      <c r="Q38" s="24"/>
+      <c r="R38" s="24"/>
+      <c r="S38" s="24"/>
+      <c r="T38" s="24"/>
       <c r="U38" s="5"/>
       <c r="V38" s="5"/>
       <c r="W38" s="5"/>
@@ -3395,26 +3457,26 @@
       <c r="AA38" s="5"/>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="22"/>
-      <c r="O39" s="22"/>
-      <c r="P39" s="22"/>
-      <c r="Q39" s="22"/>
-      <c r="R39" s="22"/>
-      <c r="S39" s="22"/>
-      <c r="T39" s="22"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="24"/>
+      <c r="N39" s="24"/>
+      <c r="O39" s="24"/>
+      <c r="P39" s="24"/>
+      <c r="Q39" s="24"/>
+      <c r="R39" s="24"/>
+      <c r="S39" s="24"/>
+      <c r="T39" s="24"/>
       <c r="U39" s="5"/>
       <c r="V39" s="5"/>
       <c r="W39" s="5"/>
@@ -3424,26 +3486,26 @@
       <c r="AA39" s="5"/>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
-      <c r="O40" s="22"/>
-      <c r="P40" s="22"/>
-      <c r="Q40" s="22"/>
-      <c r="R40" s="22"/>
-      <c r="S40" s="22"/>
-      <c r="T40" s="22"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="24"/>
+      <c r="L40" s="24"/>
+      <c r="M40" s="24"/>
+      <c r="N40" s="24"/>
+      <c r="O40" s="24"/>
+      <c r="P40" s="24"/>
+      <c r="Q40" s="24"/>
+      <c r="R40" s="24"/>
+      <c r="S40" s="24"/>
+      <c r="T40" s="24"/>
       <c r="U40" s="5"/>
       <c r="V40" s="5"/>
       <c r="W40" s="5"/>
@@ -3453,26 +3515,26 @@
       <c r="AA40" s="5"/>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="22"/>
-      <c r="L41" s="22"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="22"/>
-      <c r="O41" s="22"/>
-      <c r="P41" s="22"/>
-      <c r="Q41" s="22"/>
-      <c r="R41" s="22"/>
-      <c r="S41" s="22"/>
-      <c r="T41" s="22"/>
+      <c r="A41" s="24"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="24"/>
+      <c r="N41" s="24"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
+      <c r="Q41" s="24"/>
+      <c r="R41" s="24"/>
+      <c r="S41" s="24"/>
+      <c r="T41" s="24"/>
       <c r="U41" s="5"/>
       <c r="V41" s="5"/>
       <c r="W41" s="5"/>
@@ -3482,26 +3544,26 @@
       <c r="AA41" s="5"/>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="22"/>
-      <c r="J42" s="22"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="22"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="22"/>
-      <c r="P42" s="22"/>
-      <c r="Q42" s="22"/>
-      <c r="R42" s="22"/>
-      <c r="S42" s="22"/>
-      <c r="T42" s="22"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="24"/>
+      <c r="N42" s="24"/>
+      <c r="O42" s="24"/>
+      <c r="P42" s="24"/>
+      <c r="Q42" s="24"/>
+      <c r="R42" s="24"/>
+      <c r="S42" s="24"/>
+      <c r="T42" s="24"/>
       <c r="U42" s="5"/>
       <c r="V42" s="5"/>
       <c r="W42" s="5"/>

</xml_diff>